<commit_message>
added: Kadane's Algorithm solution
</commit_message>
<xml_diff>
--- a/450 DS Algo questions.xlsx
+++ b/450 DS Algo questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F1C939-63F5-4C61-B796-CF5DB934158F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78C5353-7217-4C01-B9A4-80D13EC903D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="21" x14ac:dyDescent="0.65"/>
@@ -1971,7 +1971,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.65">
@@ -1982,7 +1982,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.65">

</xml_diff>

<commit_message>
solved: merging sorted array without extra space
</commit_message>
<xml_diff>
--- a/450 DS Algo questions.xlsx
+++ b/450 DS Algo questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8FD085-D040-4A75-AF40-59F340EB06CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9373C4-022A-457C-893E-37EDD1EBE090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1845,7 +1845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2047,7 +2047,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
solved: spiral matrix and matrix search
</commit_message>
<xml_diff>
--- a/450 DS Algo questions.xlsx
+++ b/450 DS Algo questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9373C4-022A-457C-893E-37EDD1EBE090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE244C92-065A-4FF3-9AF4-1F52881A41E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1845,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2061,7 +2061,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
solved: Row with maximum ones in matrix
</commit_message>
<xml_diff>
--- a/450 DS Algo questions.xlsx
+++ b/450 DS Algo questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA2D6F2-F84F-4293-A0BA-DD3767D4CA2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFC1FBA-F211-4C1E-8BF2-0810096C91E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1845,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2450,7 +2450,7 @@
         <v>46</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>